<commit_message>
Range of S values changed (--> elastic values).
</commit_message>
<xml_diff>
--- a/doc/Input stress sequence.xlsx
+++ b/doc/Input stress sequence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7fa01722dbc575f3/Documenten/myR_on_GitHub/shiny/Brug1DLeaky/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_F25DC773A252ABDACC1048C0A9997A6A5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C213317-E8D9-415D-91E9-0353B312F89A}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_F25DC773A252ABDACC1048C0A9997A6A5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73FDC15C-6C81-45D5-B082-3FA12E109D71}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4032" yWindow="3720" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -369,23 +369,23 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="B3">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="B4">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>